<commit_message>
Worked on the effects doc. + Cleaned the Ninja skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Stats_and_Effect_List.xlsx
+++ b/GameDesign/Stats_and_Effect_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>STATS</t>
   </si>
@@ -205,6 +205,30 @@
   </si>
   <si>
     <t>[[Can't summon playable summoning]]</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>[[Protected Feet]]</t>
+  </si>
+  <si>
+    <t>[[Protected from glyph and field effect]]</t>
+  </si>
+  <si>
+    <t>[[Cyanide]]</t>
+  </si>
+  <si>
+    <t>Allow some of the Ninja skills to poison his target.</t>
+  </si>
+  <si>
+    <t>Ninja</t>
+  </si>
+  <si>
+    <t>[[Protection Layer]]</t>
+  </si>
+  <si>
+    <t>[[Reduces to 0 damage taken from distance]]                            Each damage reduced to 0 decrease the level by 1.</t>
   </si>
 </sst>
 </file>
@@ -422,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -515,18 +539,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -571,6 +583,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -856,7 +871,7 @@
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="13" t="s">
         <v>14</v>
@@ -1007,16 +1022,16 @@
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="G7" s="33" t="s">
+      <c r="G7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="28">
         <v>1</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="48" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1028,10 +1043,18 @@
       <c r="C8" s="6"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
@@ -1080,16 +1103,16 @@
       <c r="C12" s="6"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="35">
         <v>10</v>
       </c>
-      <c r="I12" s="39" t="s">
+      <c r="I12" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1101,16 +1124,16 @@
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="36" t="s">
         <v>55</v>
       </c>
-      <c r="G13" s="41" t="s">
+      <c r="G13" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="42">
+      <c r="H13" s="38">
         <v>10</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1164,16 +1187,16 @@
       <c r="C16" s="6"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="46">
+      <c r="H16" s="42">
         <v>10</v>
       </c>
-      <c r="I16" s="46" t="s">
+      <c r="I16" s="42" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1183,22 +1206,24 @@
       <c r="C17" s="6"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="47" t="s">
+      <c r="F17" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="43">
+      <c r="H17" s="39">
         <v>100</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="39" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="13"/>
+      <c r="B18" s="13" t="s">
+        <v>62</v>
+      </c>
       <c r="C18" s="6"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
@@ -1221,16 +1246,16 @@
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="G19" s="38" t="s">
+      <c r="G19" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="35">
         <v>100</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="35" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1240,16 +1265,16 @@
       <c r="C20" s="6"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="42">
+      <c r="H20" s="38">
         <v>100</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="39" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1297,16 +1322,16 @@
       <c r="C23" s="6"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="50" t="s">
+      <c r="G23" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="H23" s="51">
+      <c r="H23" s="47">
         <v>200</v>
       </c>
-      <c r="I23" s="51" t="s">
+      <c r="I23" s="47" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1346,21 +1371,37 @@
       <c r="C26" s="6"/>
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F26" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="H26" s="31">
+        <v>1</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="13"/>
       <c r="C27" s="6"/>
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="F27" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="6">
+        <v>3</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -1421,7 +1462,7 @@
       <c r="A33" s="1"/>
       <c r="B33" s="13"/>
       <c r="C33" s="6"/>
-      <c r="E33" s="36"/>
+      <c r="E33" s="32"/>
       <c r="F33" s="13"/>
       <c r="G33" s="16"/>
       <c r="H33" s="6"/>
@@ -1431,7 +1472,7 @@
       <c r="A34" s="1"/>
       <c r="B34" s="13"/>
       <c r="C34" s="6"/>
-      <c r="E34" s="36"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="29"/>
       <c r="G34" s="30"/>
       <c r="H34" s="31"/>
@@ -1441,7 +1482,7 @@
       <c r="A35" s="1"/>
       <c r="B35" s="13"/>
       <c r="C35" s="6"/>
-      <c r="E35" s="36"/>
+      <c r="E35" s="32"/>
       <c r="F35" s="13"/>
       <c r="G35" s="16"/>
       <c r="H35" s="6"/>
@@ -1451,7 +1492,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="13"/>
       <c r="C36" s="6"/>
-      <c r="E36" s="36"/>
+      <c r="E36" s="32"/>
       <c r="F36" s="13"/>
       <c r="G36" s="16"/>
       <c r="H36" s="6"/>
@@ -1461,7 +1502,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="13"/>
       <c r="C37" s="6"/>
-      <c r="E37" s="36"/>
+      <c r="E37" s="32"/>
       <c r="F37" s="13"/>
       <c r="G37" s="16"/>
       <c r="H37" s="6"/>
@@ -1471,7 +1512,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="13"/>
       <c r="C38" s="6"/>
-      <c r="E38" s="36"/>
+      <c r="E38" s="32"/>
       <c r="F38" s="13"/>
       <c r="G38" s="16"/>
       <c r="H38" s="6"/>
@@ -1481,7 +1522,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="13"/>
       <c r="C39" s="6"/>
-      <c r="E39" s="36"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="29"/>
       <c r="G39" s="30"/>
       <c r="H39" s="31"/>
@@ -1491,7 +1532,7 @@
       <c r="A40" s="1"/>
       <c r="B40" s="14"/>
       <c r="C40" s="7"/>
-      <c r="E40" s="36"/>
+      <c r="E40" s="32"/>
       <c r="F40" s="14"/>
       <c r="G40" s="17"/>
       <c r="H40" s="7"/>

</xml_diff>

<commit_message>
Added the notion of Undebuffable effect.
</commit_message>
<xml_diff>
--- a/GameDesign/Stats_and_Effect_List.xlsx
+++ b/GameDesign/Stats_and_Effect_List.xlsx
@@ -30,9 +30,6 @@
     <t>[[Punch]]</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -105,15 +102,6 @@
     <t>[[Weak]]</t>
   </si>
   <si>
-    <t>[[Increase the next ''Liquid Kick'' skill damage by 20%]]                  ( * effect levels )</t>
-  </si>
-  <si>
-    <t>[[Increase the next ''Iron Punch'' skill damage by 20%]]                  ( * effect levels )</t>
-  </si>
-  <si>
-    <t>Increase the damage taken by the ''Precision Strike'' skill.</t>
-  </si>
-  <si>
     <t>[[Vulnerable]]</t>
   </si>
   <si>
@@ -126,12 +114,6 @@
     <t xml:space="preserve">       [[Reduce resistance by 1%]]    ( * effect levels )</t>
   </si>
   <si>
-    <t xml:space="preserve"> [[Increase HP by 30%]]                                                                                [[Increase resistance by 15%]]</t>
-  </si>
-  <si>
-    <t>[[Increase power by 200]]                                                                            [[Increase AP by 1]]</t>
-  </si>
-  <si>
     <t>[[Increase HP by 1%]]    ( * effect levels )</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>[[Blood Mark]]</t>
   </si>
   <si>
-    <t>[[Increase the next ''Cursed Arrow'' skill damage]]                                [[Increase the ''Poison Arrow'' poison duration]]</t>
-  </si>
-  <si>
     <t>[[Poison]]</t>
   </si>
   <si>
@@ -201,9 +180,6 @@
     <t>[[Loneliness]]</t>
   </si>
   <si>
-    <t>[[Can't summon playable summoning]]</t>
-  </si>
-  <si>
     <t>Will</t>
   </si>
   <si>
@@ -216,9 +192,6 @@
     <t>[[Cyanide]]</t>
   </si>
   <si>
-    <t>Allow some of the Ninja skills to poison his target.</t>
-  </si>
-  <si>
     <t>Ninja</t>
   </si>
   <si>
@@ -231,9 +204,6 @@
     <t>[[Invulnerable]]</t>
   </si>
   <si>
-    <t>Can't loose HP</t>
-  </si>
-  <si>
     <t>Any</t>
   </si>
   <si>
@@ -252,9 +222,6 @@
     <t>[[Will Of Destruction]]</t>
   </si>
   <si>
-    <t>Prevent the usage of some skills of the Guardian.</t>
-  </si>
-  <si>
     <t>Guardian</t>
   </si>
   <si>
@@ -262,6 +229,39 @@
   </si>
   <si>
     <t>[[Increase final damage by 1%]]    ( * effect levels )</t>
+  </si>
+  <si>
+    <t>Prevent the usage of some skills of the Guardian.                       (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Increase the next ''Cursed Arrow'' skill damage]]                                [[Increase the ''Poison Arrow'' poison duration]]                             (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>Increase the damage taken by the ''Precision Strike'' skill.            (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Increase power by 200]]                                                                            [[Increase AP by 1]]                                                                                       (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [[Increase HP by 30%]]                                                                                [[Increase resistance by 15%]]                                                                                      (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>Allow some of the Ninja skills to poison his target.                                       (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>Can't loose HP                                                                                                        (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Can't summon playable summoning]]                                               (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Increase the next ''Iron Punch'' skill damage by 20%]]                  ( * effect levels )                                                                                         (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Increase the next ''Liquid Kick'' skill damage by 20%]]                  ( * effect levels )                                                                                         (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -947,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,110 +970,110 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
       <c r="F2" s="15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="H2" s="3">
         <v>1</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="H3" s="6">
         <v>1</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="H4" s="6">
         <v>5</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="H5" s="6">
         <v>2</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="4"/>
@@ -1082,82 +1082,82 @@
         <v>2</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="H7" s="27">
         <v>1</v>
       </c>
       <c r="I7" s="47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5"/>
       <c r="F8" s="25" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="H8" s="27">
         <v>1</v>
       </c>
       <c r="I8" s="47" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
       <c r="F9" s="25" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="G9" s="26" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="H9" s="27">
         <v>1</v>
       </c>
       <c r="I9" s="47" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="4"/>
@@ -1170,7 +1170,7 @@
     <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="4"/>
@@ -1183,106 +1183,106 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="4"/>
       <c r="E12" s="5"/>
       <c r="F12" s="32" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G12" s="33" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H12" s="34">
         <v>10</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="4"/>
       <c r="E13" s="5"/>
       <c r="F13" s="35" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H13" s="37">
         <v>10</v>
       </c>
       <c r="I13" s="38" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
       <c r="F14" s="15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3">
         <v>10</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
       <c r="F15" s="13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H15" s="6">
         <v>10</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
       <c r="F16" s="51" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H16" s="21">
         <v>1</v>
       </c>
       <c r="I16" s="21" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,37 +1292,37 @@
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
       <c r="F17" s="39" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="H17" s="41">
         <v>10</v>
       </c>
       <c r="I17" s="41" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="13" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
       <c r="F18" s="42" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G18" s="36" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H18" s="38">
         <v>100</v>
       </c>
       <c r="I18" s="38" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1332,35 +1332,35 @@
       <c r="D19" s="4"/>
       <c r="E19" s="5"/>
       <c r="F19" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G19" s="26" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H19" s="27">
         <v>100</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="13"/>
       <c r="C20" s="6"/>
       <c r="D20" s="4"/>
       <c r="E20" s="5"/>
       <c r="F20" s="53" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="H20" s="55">
         <v>1</v>
       </c>
       <c r="I20" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1370,16 +1370,16 @@
       <c r="D21" s="4"/>
       <c r="E21" s="5"/>
       <c r="F21" s="57" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G21" s="58" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H21" s="59">
         <v>100</v>
       </c>
       <c r="I21" s="59" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1389,16 +1389,16 @@
       <c r="D22" s="4"/>
       <c r="E22" s="5"/>
       <c r="F22" s="53" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H22" s="55">
         <v>100</v>
       </c>
       <c r="I22" s="56" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1408,16 +1408,16 @@
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
       <c r="F23" s="57" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="H23" s="59">
         <v>3</v>
       </c>
       <c r="I23" s="59" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1427,16 +1427,16 @@
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
       <c r="F24" s="53" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="H24" s="55">
         <v>1</v>
       </c>
       <c r="I24" s="55" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,16 +1446,16 @@
       <c r="D25" s="4"/>
       <c r="E25" s="5"/>
       <c r="F25" s="35" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G25" s="43" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="H25" s="37">
         <v>100</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1465,16 +1465,16 @@
       <c r="D26" s="4"/>
       <c r="E26" s="5"/>
       <c r="F26" s="48" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="G26" s="49" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="H26" s="50">
         <v>100</v>
       </c>
       <c r="I26" s="50" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1484,16 +1484,16 @@
       <c r="D27" s="4"/>
       <c r="E27" s="5"/>
       <c r="F27" s="13" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H27" s="52">
         <v>1000</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1503,16 +1503,16 @@
       <c r="D28" s="4"/>
       <c r="E28" s="5"/>
       <c r="F28" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H28" s="23">
         <v>1000</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1522,35 +1522,35 @@
       <c r="D29" s="4"/>
       <c r="E29" s="5"/>
       <c r="F29" s="44" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G29" s="45" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H29" s="46">
         <v>100</v>
       </c>
       <c r="I29" s="46" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="13"/>
       <c r="C30" s="6"/>
       <c r="D30" s="4"/>
       <c r="E30" s="5"/>
       <c r="F30" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="H30" s="8">
         <v>1</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished the effects doc, but still need to clean the effects names, do the glyph doc and finish the stats doc. + Cleaned the Cyborg skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Stats_and_Effect_List.xlsx
+++ b/GameDesign/Stats_and_Effect_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="160">
   <si>
     <t>STATS</t>
   </si>
@@ -753,6 +753,27 @@
   </si>
   <si>
     <t>All skills damage steal life, they steal ratio increase by 100%                                                                                     (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>Cyborg</t>
+  </si>
+  <si>
+    <t>[[Power Supply]]</t>
+  </si>
+  <si>
+    <t>Allow the usage of some Cyborg skills                                                         (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Self-Destruction Countdown]]</t>
+  </si>
+  <si>
+    <t>When effect is removed, entity K/O.                                                                      (Can't be unbuffed)</t>
+  </si>
+  <si>
+    <t>[[Checkpoint]]</t>
+  </si>
+  <si>
+    <t>Save the position when gaining this effect.                                              Teleport to the saved position at the end of the turn and remove the ''Checkpoint Glyph''                                                                     If can't be teleported: [[Damage: 100 light]]</t>
   </si>
 </sst>
 </file>
@@ -1458,8 +1479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="C76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,7 +1490,7 @@
     <col min="3" max="3" width="7.28515625" customWidth="1"/>
     <col min="4" max="4" width="3.7109375" customWidth="1"/>
     <col min="5" max="5" width="0.42578125" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
     <col min="7" max="7" width="54.85546875" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
@@ -2028,7 +2049,7 @@
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
     </row>
-    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="13" t="s">
         <v>124</v>
@@ -2036,24 +2057,26 @@
       <c r="C23" s="6"/>
       <c r="D23" s="4"/>
       <c r="E23" s="5"/>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="7">
         <v>1</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="J23" s="18"/>
+      <c r="J23" s="22" t="s">
+        <v>141</v>
+      </c>
       <c r="O23" s="13"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="13" t="s">
         <v>125</v>
@@ -2061,11 +2084,19 @@
       <c r="C24" s="6"/>
       <c r="D24" s="4"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6"/>
+      <c r="F24" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H24" s="8">
+        <v>20</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="J24" s="18"/>
       <c r="O24" s="13"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
@@ -3140,27 +3171,47 @@
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="13"/>
       <c r="C85" s="6"/>
       <c r="E85" s="31"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="29"/>
-      <c r="H85" s="30"/>
-      <c r="I85" s="30"/>
-      <c r="J85" s="30"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F85" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="G85" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="H85" s="30">
+        <v>1</v>
+      </c>
+      <c r="I85" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="J85" s="30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="13"/>
       <c r="C86" s="6"/>
       <c r="E86" s="31"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
-      <c r="J86" s="6"/>
+      <c r="F86" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G86" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="H86" s="6">
+        <v>1</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="J86" s="6" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>

</xml_diff>

<commit_message>
Finished listing character stats.
</commit_message>
<xml_diff>
--- a/GameDesign/Stats_and_Effect_List.xlsx
+++ b/GameDesign/Stats_and_Effect_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="3" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="206">
   <si>
     <t>STATS</t>
   </si>
@@ -50,12 +50,6 @@
     <t>[[Fighter Meditation]]</t>
   </si>
   <si>
-    <t>HP by %</t>
-  </si>
-  <si>
-    <t>Resistance by %</t>
-  </si>
-  <si>
     <t>Final damage by %</t>
   </si>
   <si>
@@ -77,18 +71,6 @@
     <t>Ground damage</t>
   </si>
   <si>
-    <t>Fire resistance</t>
-  </si>
-  <si>
-    <t>Water resistance</t>
-  </si>
-  <si>
-    <t>Wind resistance</t>
-  </si>
-  <si>
-    <t>Ground resistance</t>
-  </si>
-  <si>
     <t>AP</t>
   </si>
   <si>
@@ -240,9 +222,6 @@
   </si>
   <si>
     <t>[[Increase the next ''Liquid Kick'' skill damage by 20%]]                  ( * effect levels )                                                                                         (Can't be unbuffed)</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Elementalist</t>
@@ -470,12 +449,6 @@
     <t>Increase the damage taken by the ''Katana'' skill.</t>
   </si>
   <si>
-    <t>Melee Damage by %</t>
-  </si>
-  <si>
-    <t>Ranged Damage by %</t>
-  </si>
-  <si>
     <t>[[Melee]]</t>
   </si>
   <si>
@@ -1167,6 +1140,45 @@
   </si>
   <si>
     <t>Just a visual indication.</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Fire resistance by %</t>
+  </si>
+  <si>
+    <t>Water resistance by %</t>
+  </si>
+  <si>
+    <t>Wind resistance by %</t>
+  </si>
+  <si>
+    <t>Ground resistance by %</t>
+  </si>
+  <si>
+    <t>Initial Max HP</t>
+  </si>
+  <si>
+    <t>Light damage</t>
+  </si>
+  <si>
+    <t>Dark damage</t>
+  </si>
+  <si>
+    <t>Light resistance by %</t>
+  </si>
+  <si>
+    <t>Dark resistance by %</t>
+  </si>
+  <si>
+    <t>Reflecting damage by %</t>
+  </si>
+  <si>
+    <t>Melee final Damage by %</t>
+  </si>
+  <si>
+    <t>Ranged final Damage by %</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1574,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1961,6 +1973,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2254,523 +2269,205 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.42578125" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="135" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="34" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="12"/>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="12"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="12"/>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="12"/>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="12"/>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="12"/>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="12"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="12"/>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="12"/>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="5"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="5"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="5"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="5"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="5"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="5"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="5"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="5"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="5"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="5"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="12"/>
-      <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="12"/>
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="12"/>
-      <c r="C50" s="5"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="5"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="5"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="5"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="5"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="5"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="12"/>
-      <c r="C56" s="5"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="5"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="5"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="5"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="5"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="5"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="12"/>
-      <c r="C62" s="5"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="5"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="12"/>
-      <c r="C64" s="5"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="5"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="12"/>
-      <c r="C67" s="5"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="5"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="5"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="5"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="5"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="5"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="5"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="5"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="5"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="12"/>
-      <c r="C78" s="5"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="12"/>
-      <c r="C79" s="5"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="5"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="12"/>
-      <c r="C81" s="5"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="5"/>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="5"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="5"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="12"/>
-      <c r="C85" s="5"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="12"/>
-      <c r="C86" s="5"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="12"/>
-      <c r="C87" s="5"/>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="5"/>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="12"/>
-      <c r="C89" s="5"/>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="12"/>
-      <c r="C90" s="5"/>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="12"/>
-      <c r="C91" s="5"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="12"/>
-      <c r="C92" s="5"/>
-    </row>
-    <row r="93" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1"/>
-      <c r="B93" s="13"/>
-      <c r="C93" s="6"/>
+      <c r="B35" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2781,7 +2478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
@@ -2810,7 +2507,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -2819,7 +2516,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -2832,10 +2529,10 @@
     <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
@@ -2848,10 +2545,10 @@
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="12" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D4" s="5">
         <v>5</v>
@@ -2864,10 +2561,10 @@
     <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D5" s="5">
         <v>2</v>
@@ -2883,7 +2580,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D6" s="6">
         <v>2</v>
@@ -2896,290 +2593,290 @@
     <row r="7" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D7" s="32">
         <v>1</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="21" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D8" s="23">
         <v>1</v>
       </c>
       <c r="E8" s="33" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="B9" s="30" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D9" s="32">
         <v>1</v>
       </c>
       <c r="E9" s="33" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="34" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D10" s="36">
         <v>5</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="12" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D11" s="5">
         <v>5</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="12" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D12" s="5">
         <v>5</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="12" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="D13" s="5">
         <v>5</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="12" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="13" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="40" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C16" s="27" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D16" s="28">
         <v>1</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="37" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D17" s="39">
         <v>1</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="25" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D18" s="26">
         <v>1</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D19" s="7">
         <v>1</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F19" s="17"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="12" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F20" s="17"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="D21" s="6">
         <v>3</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="40" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C22" s="27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D22" s="28">
         <v>50</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F22" s="17"/>
     </row>
     <row r="23" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="25" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D23" s="26">
         <v>1</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="F23" s="20" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="21" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D24" s="23">
         <v>20</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="F24" s="33"/>
     </row>
@@ -3192,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3230,49 +2927,49 @@
         <v>4</v>
       </c>
       <c r="E1" s="41" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="F1" s="41"/>
       <c r="G1" s="112" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="K1" s="41" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="L1" s="112" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="M1" s="112" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="N1" s="41" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="O1" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="P1" s="41" t="s">
         <v>133</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>142</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="S1" s="132" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="42"/>
       <c r="C2" s="45" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D2" s="43"/>
       <c r="E2" s="44"/>
@@ -3282,7 +2979,7 @@
       <c r="I2" s="120"/>
       <c r="J2" s="120"/>
       <c r="K2" s="45" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="L2" s="120"/>
       <c r="M2" s="120"/>
@@ -3291,16 +2988,16 @@
       <c r="P2" s="120"/>
       <c r="Q2" s="1"/>
       <c r="S2" s="133" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="24"/>
       <c r="B3" s="82" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C3" s="83" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D3" s="84">
         <v>10</v>
@@ -3327,16 +3024,16 @@
       </c>
       <c r="Q3" s="1"/>
       <c r="S3" s="134" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24"/>
       <c r="B4" s="66" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D4" s="68">
         <v>10</v>
@@ -3362,16 +3059,16 @@
     <row r="5" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24"/>
       <c r="B5" s="66" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C5" s="70" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D5" s="68">
         <v>1</v>
       </c>
       <c r="E5" s="68" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F5" s="109"/>
       <c r="G5" s="122"/>
@@ -3391,16 +3088,16 @@
     <row r="6" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24"/>
       <c r="B6" s="71" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C6" s="72" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6" s="73">
         <v>1</v>
       </c>
       <c r="E6" s="73" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F6" s="109"/>
       <c r="G6" s="122"/>
@@ -3438,7 +3135,7 @@
       <c r="A8" s="24"/>
       <c r="B8" s="46"/>
       <c r="C8" s="47" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="49"/>
@@ -3448,7 +3145,7 @@
       <c r="I8" s="126"/>
       <c r="J8" s="126"/>
       <c r="K8" s="47" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="L8" s="126"/>
       <c r="M8" s="126"/>
@@ -3460,10 +3157,10 @@
     <row r="9" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24"/>
       <c r="B9" s="82" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C9" s="83" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D9" s="84">
         <v>10</v>
@@ -3493,10 +3190,10 @@
     <row r="10" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24"/>
       <c r="B10" s="74" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D10" s="76">
         <v>10</v>
@@ -3526,16 +3223,16 @@
     <row r="11" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="99" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C11" s="100" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D11" s="101">
         <v>1</v>
       </c>
       <c r="E11" s="101" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F11" s="109"/>
       <c r="G11" s="127"/>
@@ -3561,16 +3258,16 @@
     <row r="12" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="24"/>
       <c r="B12" s="102" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C12" s="103" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D12" s="104">
         <v>1</v>
       </c>
       <c r="E12" s="104" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F12" s="109"/>
       <c r="G12" s="127"/>
@@ -3590,16 +3287,16 @@
     <row r="13" spans="1:19" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24"/>
       <c r="B13" s="105" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C13" s="106" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D13" s="107">
         <v>1</v>
       </c>
       <c r="E13" s="107" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F13" s="109"/>
       <c r="G13" s="127"/>
@@ -3639,7 +3336,7 @@
       <c r="A15" s="24"/>
       <c r="B15" s="113"/>
       <c r="C15" s="114" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D15" s="115"/>
       <c r="E15" s="116"/>
@@ -3649,7 +3346,7 @@
       <c r="I15" s="128"/>
       <c r="J15" s="128"/>
       <c r="K15" s="114" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="L15" s="128"/>
       <c r="M15" s="128"/>
@@ -3661,10 +3358,10 @@
     <row r="16" spans="1:19" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24"/>
       <c r="B16" s="85" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C16" s="83" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D16" s="84">
         <v>10</v>
@@ -3686,10 +3383,10 @@
     <row r="17" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24"/>
       <c r="B17" s="77" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C17" s="78" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D17" s="79">
         <v>100</v>
@@ -3737,7 +3434,7 @@
       <c r="A19" s="24"/>
       <c r="B19" s="50"/>
       <c r="C19" s="51" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="D19" s="52"/>
       <c r="E19" s="53"/>
@@ -3747,7 +3444,7 @@
       <c r="I19" s="129"/>
       <c r="J19" s="129"/>
       <c r="K19" s="51" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L19" s="129"/>
       <c r="M19" s="129"/>
@@ -3759,10 +3456,10 @@
     <row r="20" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
       <c r="B20" s="86" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C20" s="87" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D20" s="88">
         <v>100</v>
@@ -3790,10 +3487,10 @@
     <row r="21" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24"/>
       <c r="B21" s="66" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C21" s="70" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D21" s="68">
         <v>100</v>
@@ -3817,16 +3514,16 @@
     <row r="22" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24"/>
       <c r="B22" s="74" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C22" s="75" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D22" s="76">
         <v>1</v>
       </c>
       <c r="E22" s="76" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F22" s="109"/>
       <c r="G22" s="122"/>
@@ -3846,16 +3543,16 @@
     <row r="23" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24"/>
       <c r="B23" s="102" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C23" s="103" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D23" s="104">
         <v>1</v>
       </c>
       <c r="E23" s="104" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F23" s="109"/>
       <c r="G23" s="127"/>
@@ -3877,16 +3574,16 @@
     <row r="24" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24"/>
       <c r="B24" s="74" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C24" s="75" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D24" s="76">
         <v>1</v>
       </c>
       <c r="E24" s="76" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F24" s="109"/>
       <c r="G24" s="122"/>
@@ -3908,16 +3605,16 @@
     <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24"/>
       <c r="B25" s="71" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C25" s="72" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="D25" s="73">
         <v>1</v>
       </c>
       <c r="E25" s="73" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F25" s="109"/>
       <c r="G25" s="122"/>
@@ -3957,7 +3654,7 @@
       <c r="A27" s="24"/>
       <c r="B27" s="54"/>
       <c r="C27" s="55" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D27" s="56"/>
       <c r="E27" s="57"/>
@@ -3967,7 +3664,7 @@
       <c r="I27" s="130"/>
       <c r="J27" s="130"/>
       <c r="K27" s="55" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="L27" s="130"/>
       <c r="M27" s="130"/>
@@ -3979,16 +3676,16 @@
     <row r="28" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24"/>
       <c r="B28" s="86" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C28" s="87" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D28" s="88">
         <v>1</v>
       </c>
       <c r="E28" s="88" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F28" s="109"/>
       <c r="G28" s="121"/>
@@ -4012,16 +3709,16 @@
     <row r="29" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24"/>
       <c r="B29" s="89" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C29" s="90" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D29" s="91">
         <v>1</v>
       </c>
       <c r="E29" s="91" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F29" s="109"/>
       <c r="G29" s="121"/>
@@ -4043,16 +3740,16 @@
     <row r="30" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24"/>
       <c r="B30" s="89" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C30" s="90" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="D30" s="92">
         <v>1</v>
       </c>
       <c r="E30" s="92" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F30" s="109"/>
       <c r="G30" s="121"/>
@@ -4070,10 +3767,10 @@
     <row r="31" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24"/>
       <c r="B31" s="93" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C31" s="94" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D31" s="92">
         <v>100</v>
@@ -4099,10 +3796,10 @@
     <row r="32" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24"/>
       <c r="B32" s="66" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C32" s="70" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D32" s="68">
         <v>100</v>
@@ -4134,10 +3831,10 @@
     <row r="33" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24"/>
       <c r="B33" s="66" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C33" s="70" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D33" s="68">
         <v>100</v>
@@ -4159,10 +3856,10 @@
     <row r="34" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24"/>
       <c r="B34" s="74" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C34" s="75" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D34" s="76">
         <v>100</v>
@@ -4184,10 +3881,10 @@
     <row r="35" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24"/>
       <c r="B35" s="102" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C35" s="103" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D35" s="104">
         <v>50</v>
@@ -4211,16 +3908,16 @@
     <row r="36" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24"/>
       <c r="B36" s="93" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C36" s="94" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D36" s="92">
         <v>3</v>
       </c>
       <c r="E36" s="92" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F36" s="109"/>
       <c r="G36" s="121"/>
@@ -4242,16 +3939,16 @@
     <row r="37" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24"/>
       <c r="B37" s="117" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C37" s="118" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D37" s="119">
         <v>1</v>
       </c>
       <c r="E37" s="119" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F37" s="109"/>
       <c r="G37" s="127"/>
@@ -4271,16 +3968,16 @@
     <row r="38" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="24"/>
       <c r="B38" s="95" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C38" s="96" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D38" s="97">
         <v>100</v>
       </c>
       <c r="E38" s="97" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F38" s="109"/>
       <c r="G38" s="121"/>
@@ -4320,7 +4017,7 @@
       <c r="A40" s="24"/>
       <c r="B40" s="58"/>
       <c r="C40" s="59" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D40" s="60"/>
       <c r="E40" s="61"/>
@@ -4330,7 +4027,7 @@
       <c r="I40" s="131"/>
       <c r="J40" s="131"/>
       <c r="K40" s="59" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="L40" s="131"/>
       <c r="M40" s="131"/>
@@ -4342,10 +4039,10 @@
     <row r="41" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24"/>
       <c r="B41" s="86" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C41" s="87" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D41" s="88">
         <v>100</v>
@@ -4373,10 +4070,10 @@
     <row r="42" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24"/>
       <c r="B42" s="80" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D42" s="76">
         <v>100</v>
@@ -4400,10 +4097,10 @@
     <row r="43" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24"/>
       <c r="B43" s="93" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C43" s="94" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D43" s="92">
         <v>100</v>
@@ -4427,10 +4124,10 @@
     <row r="44" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24"/>
       <c r="B44" s="93" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C44" s="94" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D44" s="92">
         <v>100</v>
@@ -4454,10 +4151,10 @@
     <row r="45" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24"/>
       <c r="B45" s="93" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C45" s="94" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D45" s="92">
         <v>100</v>
@@ -4481,10 +4178,10 @@
     <row r="46" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24"/>
       <c r="B46" s="93" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C46" s="94" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D46" s="98">
         <v>1000</v>
@@ -4506,10 +4203,10 @@
     <row r="47" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24"/>
       <c r="B47" s="66" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C47" s="70" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D47" s="81">
         <v>1000</v>
@@ -4535,10 +4232,10 @@
     <row r="48" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24"/>
       <c r="B48" s="74" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C48" s="75" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D48" s="76">
         <v>100</v>
@@ -4566,16 +4263,16 @@
     <row r="49" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24"/>
       <c r="B49" s="71" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C49" s="72" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="D49" s="73">
         <v>100</v>
       </c>
       <c r="E49" s="73" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F49" s="111"/>
       <c r="G49" s="122"/>
@@ -4636,182 +4333,182 @@
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="12" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="12" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="12" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="12" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="12" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="12" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C9" s="5">
         <f>-C16</f>
         <v>0</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="12" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="12" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="11" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="12" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="12" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="12" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -5083,12 +4780,12 @@
   <sheetData>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>